<commit_message>
update main.py adn analyzing_data.py
</commit_message>
<xml_diff>
--- a/outputs/regression_results.xlsx
+++ b/outputs/regression_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.729</t>
+          <t>0.026</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -557,7 +557,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>29.9829</t>
+          <t>61.1308</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-02-24 01:02</t>
+          <t>2025-02-24 21:53</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -588,7 +588,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>34.8584</t>
+          <t>64.7875</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -619,7 +619,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-10.991</t>
+          <t>-27.565</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -640,7 +640,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>22.52</t>
+          <t>1.320</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -671,7 +671,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>9.16e-07</t>
+          <t>0.287</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.763</t>
+          <t>0.107</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -712,7 +712,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.16793</t>
+          <t>0.60362</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -736,22 +736,22 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>-4.488367156397095</v>
+        <v>1.889356166716446</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9755853017823947</v>
+        <v>1.223072791961466</v>
       </c>
       <c r="I10" t="n">
-        <v>-4.600691654739823</v>
+        <v>1.544761831948242</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0001546352537605774</v>
+        <v>0.1366680517385894</v>
       </c>
       <c r="K10" t="n">
-        <v>-6.517207856696577</v>
+        <v>-0.6471415566186085</v>
       </c>
       <c r="L10" t="n">
-        <v>-2.459526456097612</v>
+        <v>4.425853890051501</v>
       </c>
       <c r="M10" t="inlineStr"/>
     </row>
@@ -763,29 +763,29 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>平均気温(℃)_4_下旬</t>
+          <t>平均気温(℃)_1_上旬</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0.1915057525007337</v>
+        <v>-0.3160093911476233</v>
       </c>
       <c r="H11" t="n">
-        <v>0.05381629016720139</v>
+        <v>0.2663557556451867</v>
       </c>
       <c r="I11" t="n">
-        <v>3.558508992458343</v>
+        <v>-1.186418481486018</v>
       </c>
       <c r="J11" t="n">
-        <v>0.001857197708189514</v>
+        <v>0.2481119774298942</v>
       </c>
       <c r="K11" t="n">
-        <v>0.07958865039714048</v>
+        <v>-0.8683974192613986</v>
       </c>
       <c r="L11" t="n">
-        <v>0.3034228546043268</v>
+        <v>0.236378636966152</v>
       </c>
       <c r="M11" t="n">
-        <v>0.3853869628902444</v>
+        <v>-0.5107291395604036</v>
       </c>
     </row>
     <row r="12">
@@ -796,29 +796,29 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>日最高気温の平均(℃)_1_中旬</t>
+          <t>日最低気温の平均(℃)_1_上旬</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0.1656552634562546</v>
+        <v>0.3912088139128793</v>
       </c>
       <c r="H12" t="n">
-        <v>0.05772178324513121</v>
+        <v>0.2494758819424517</v>
       </c>
       <c r="I12" t="n">
-        <v>2.869891644767012</v>
+        <v>1.5681227815165</v>
       </c>
       <c r="J12" t="n">
-        <v>0.009168194065138335</v>
+        <v>0.1311245686452912</v>
       </c>
       <c r="K12" t="n">
-        <v>0.04561624387731052</v>
+        <v>-0.1261724987391728</v>
       </c>
       <c r="L12" t="n">
-        <v>0.2856942830351987</v>
+        <v>0.9085901265649314</v>
       </c>
       <c r="M12" t="n">
-        <v>0.312417841616266</v>
+        <v>0.6750451138672922</v>
       </c>
     </row>
     <row r="13">
@@ -827,428 +827,14 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>日最低気温の平均(℃)_1_下旬</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>0.43138041026291</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.06694508164267994</v>
-      </c>
-      <c r="I13" t="n">
-        <v>6.443795416747825</v>
-      </c>
-      <c r="J13" t="n">
-        <v>2.189505814400155e-06</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.2921604916423691</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.5706003288834508</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.7084335814712248</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Best2</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Model:</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>OLS</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Adj. R-squared:</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>0.687</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Dependent Variable:</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>発病率</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>AIC:</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>33.5517</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Date:</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2025-02-24 01:02</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>BIC:</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>38.4272</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>No. Observations:</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Log-Likelihood:</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>-12.776</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Df Model:</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>F-statistic:</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>18.60</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Df Residuals:</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Prob (F-statistic):</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>4.01e-06</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>R-squared:</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>0.727</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Scale:</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>0.19370</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>const</t>
-        </is>
-      </c>
-      <c r="G23" t="n">
-        <v>-3.450274858657991</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.9379734148112036</v>
-      </c>
-      <c r="I23" t="n">
-        <v>-3.678435661582654</v>
-      </c>
-      <c r="J23" t="n">
-        <v>0.001397879783702184</v>
-      </c>
-      <c r="K23" t="n">
-        <v>-5.400897358085853</v>
-      </c>
-      <c r="L23" t="n">
-        <v>-1.49965235923013</v>
-      </c>
-      <c r="M23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>平均気温(℃)_1_中旬</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
-        <v>0.1764849364083666</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.08464786828717882</v>
-      </c>
-      <c r="I24" t="n">
-        <v>2.084930666057871</v>
-      </c>
-      <c r="J24" t="n">
-        <v>0.04946820310757518</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0.0004500575916659144</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0.3525198152250674</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0.2646267102789007</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>平均気温(℃)_4_下旬</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
-        <v>0.1648783656538122</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.06115255368082748</v>
-      </c>
-      <c r="I25" t="n">
-        <v>2.696181201432063</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0.01352387920233384</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0.03770466837871178</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0.2920520629289126</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0.3318019002347538</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>日最低気温の平均(℃)_1_下旬</t>
-        </is>
-      </c>
-      <c r="G26" t="n">
-        <v>0.4153406184311692</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.07520224956236303</v>
-      </c>
-      <c r="I26" t="n">
-        <v>5.522981305057096</v>
-      </c>
-      <c r="J26" t="n">
-        <v>1.762889584589413e-05</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0.2589489790866143</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0.5717322577757241</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0.6820922666987538</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add filter.py and corretion function
</commit_message>
<xml_diff>
--- a/outputs/regression_results.xlsx
+++ b/outputs/regression_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.026</t>
+          <t>0.729</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -557,7 +557,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>61.1308</t>
+          <t>29.9829</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-02-24 21:53</t>
+          <t>2025-02-25 01:14</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -588,7 +588,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>64.7875</t>
+          <t>34.8584</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -619,7 +619,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-27.565</t>
+          <t>-10.991</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -640,7 +640,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.320</t>
+          <t>22.52</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -671,7 +671,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.287</t>
+          <t>9.16e-07</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.107</t>
+          <t>0.763</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -712,7 +712,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.60362</t>
+          <t>0.16793</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -736,22 +736,22 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1.889356166716446</v>
+        <v>-4.488367156397095</v>
       </c>
       <c r="H10" t="n">
-        <v>1.223072791961466</v>
+        <v>0.9755853017823947</v>
       </c>
       <c r="I10" t="n">
-        <v>1.544761831948242</v>
+        <v>-4.600691654739823</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1366680517385894</v>
+        <v>0.0001546352537605774</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.6471415566186085</v>
+        <v>-6.517207856696577</v>
       </c>
       <c r="L10" t="n">
-        <v>4.425853890051501</v>
+        <v>-2.459526456097612</v>
       </c>
       <c r="M10" t="inlineStr"/>
     </row>
@@ -763,29 +763,29 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>平均気温(℃)_1_上旬</t>
+          <t>平均気温(℃)_4_下旬</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>-0.3160093911476233</v>
+        <v>0.1915057525007337</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2663557556451867</v>
+        <v>0.05381629016720139</v>
       </c>
       <c r="I11" t="n">
-        <v>-1.186418481486018</v>
+        <v>3.558508992458343</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2481119774298942</v>
+        <v>0.001857197708189514</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.8683974192613986</v>
+        <v>0.07958865039714048</v>
       </c>
       <c r="L11" t="n">
-        <v>0.236378636966152</v>
+        <v>0.3034228546043268</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.5107291395604036</v>
+        <v>0.3853869628902444</v>
       </c>
     </row>
     <row r="12">
@@ -796,29 +796,29 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>日最低気温の平均(℃)_1_上旬</t>
+          <t>日最高気温の平均(℃)_1_中旬</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0.3912088139128793</v>
+        <v>0.1656552634562546</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2494758819424517</v>
+        <v>0.05772178324513121</v>
       </c>
       <c r="I12" t="n">
-        <v>1.5681227815165</v>
+        <v>2.869891644767012</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1311245686452912</v>
+        <v>0.009168194065138335</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.1261724987391728</v>
+        <v>0.04561624387731052</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9085901265649314</v>
+        <v>0.2856942830351987</v>
       </c>
       <c r="M12" t="n">
-        <v>0.6750451138672922</v>
+        <v>0.312417841616266</v>
       </c>
     </row>
     <row r="13">
@@ -827,14 +827,428 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>日最低気温の平均(℃)_1_下旬</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0.43138041026291</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.06694508164267994</v>
+      </c>
+      <c r="I13" t="n">
+        <v>6.443795416747825</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2.189505814400155e-06</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.2921604916423691</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.5706003288834508</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.7084335814712248</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Best2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Model:</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>OLS</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Adj. R-squared:</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0.687</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Dependent Variable:</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>発病率</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>AIC:</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>33.5517</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Date:</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-02-25 01:14</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>BIC:</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>38.4272</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>No. Observations:</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Log-Likelihood:</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-12.776</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Df Model:</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>F-statistic:</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>18.60</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Df Residuals:</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Prob (F-statistic):</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>4.01e-06</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>R-squared:</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.727</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Scale:</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.19370</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>const</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>-3.450274858657991</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.9379734148112036</v>
+      </c>
+      <c r="I23" t="n">
+        <v>-3.678435661582654</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.001397879783702184</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-5.400897358085853</v>
+      </c>
+      <c r="L23" t="n">
+        <v>-1.49965235923013</v>
+      </c>
+      <c r="M23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>平均気温(℃)_1_中旬</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>0.1764849364083666</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.08464786828717882</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2.084930666057871</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.04946820310757518</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.0004500575916659144</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.3525198152250674</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.2646267102789007</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>平均気温(℃)_4_下旬</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1648783656538122</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.06115255368082748</v>
+      </c>
+      <c r="I25" t="n">
+        <v>2.696181201432063</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.01352387920233384</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.03770466837871178</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.2920520629289126</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.3318019002347538</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>日最低気温の平均(℃)_1_下旬</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>0.4153406184311692</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.07520224956236303</v>
+      </c>
+      <c r="I26" t="n">
+        <v>5.522981305057096</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1.762889584589413e-05</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.2589489790866143</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.5717322577757241</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.6820922666987538</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>